<commit_message>
small formatting changes to figs
</commit_message>
<xml_diff>
--- a/tables/bael_analysis_tables_151203.xlsx
+++ b/tables/bael_analysis_tables_151203.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14620" yWindow="4360" windowWidth="15360" windowHeight="15760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14560" yWindow="1160" windowWidth="23340" windowHeight="17680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AIC" sheetId="1" r:id="rId1"/>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:R12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2165,13 +2165,13 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18">
-        <v>-228.372897039099</v>
+        <v>-226.780339658477</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2180,25 +2180,25 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0.37224870457229597</v>
+        <v>0.37616564160315302</v>
       </c>
       <c r="H18">
-        <v>118.32437955403201</v>
+        <v>118.598503162572</v>
       </c>
       <c r="I18">
-        <v>0.37224870457229597</v>
+        <v>0.37616564160315302</v>
       </c>
       <c r="K18" s="10" t="str">
         <f t="shared" ref="K18:L22" si="21">B18</f>
-        <v>Size</v>
+        <v>Era + Size</v>
       </c>
       <c r="L18" s="11">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M18" s="11">
         <f t="shared" ref="M18:N22" si="22">ROUND(D18, 2)</f>
-        <v>-228.37</v>
+        <v>-226.78</v>
       </c>
       <c r="N18" s="11">
         <f t="shared" si="22"/>
@@ -2210,15 +2210,15 @@
       </c>
       <c r="P18" s="11">
         <f t="shared" si="23"/>
-        <v>0.372</v>
+        <v>0.376</v>
       </c>
       <c r="Q18" s="11">
         <f t="shared" ref="Q18:R22" si="24">ROUND(H18, 2)</f>
-        <v>118.32</v>
+        <v>118.6</v>
       </c>
       <c r="R18" s="11">
         <f t="shared" si="24"/>
-        <v>0.37</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -2226,60 +2226,60 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>-228.307659898054</v>
+        <v>-226.449966192132</v>
       </c>
       <c r="E19">
-        <v>6.5237141045628305E-2</v>
+        <v>0.33037346634500903</v>
       </c>
       <c r="F19">
-        <v>0.96790767770776398</v>
+        <v>0.84773538898840595</v>
       </c>
       <c r="G19">
-        <v>0.36030237917229502</v>
+        <v>0.31888892650852202</v>
       </c>
       <c r="H19">
-        <v>119.36216328236</v>
+        <v>117.362914130549</v>
       </c>
       <c r="I19">
-        <v>0.73255108374459099</v>
+        <v>0.69505456811167499</v>
       </c>
       <c r="K19" s="10" t="str">
         <f t="shared" si="21"/>
-        <v>Era + Size</v>
+        <v>Size</v>
       </c>
       <c r="L19" s="11">
         <f t="shared" si="21"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M19" s="11">
         <f t="shared" si="22"/>
-        <v>-228.31</v>
+        <v>-226.45</v>
       </c>
       <c r="N19" s="11">
         <f t="shared" si="22"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.33</v>
       </c>
       <c r="O19" s="11">
         <f t="shared" si="23"/>
-        <v>0.96799999999999997</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="P19" s="11">
         <f t="shared" si="23"/>
-        <v>0.36</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="Q19" s="11">
         <f t="shared" si="24"/>
-        <v>119.36</v>
+        <v>117.36</v>
       </c>
       <c r="R19" s="11">
         <f t="shared" si="24"/>
-        <v>0.73</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -2293,19 +2293,19 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>-227.71162981763101</v>
+        <v>-226.36054619087301</v>
       </c>
       <c r="E20">
-        <v>0.66126722146847805</v>
+        <v>0.41979346760339797</v>
       </c>
       <c r="F20">
-        <v>0.71846835991733304</v>
+        <v>0.810667956245818</v>
       </c>
       <c r="G20">
-        <v>0.26744891625540901</v>
+        <v>0.30494543188832501</v>
       </c>
       <c r="H20">
-        <v>120.149521202522</v>
+        <v>119.473979389143</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -2320,23 +2320,23 @@
       </c>
       <c r="M20" s="11">
         <f t="shared" si="22"/>
-        <v>-227.71</v>
+        <v>-226.36</v>
       </c>
       <c r="N20" s="11">
         <f t="shared" si="22"/>
-        <v>0.66</v>
+        <v>0.42</v>
       </c>
       <c r="O20" s="11">
         <f t="shared" si="23"/>
-        <v>0.71799999999999997</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="P20" s="11">
         <f t="shared" si="23"/>
-        <v>0.26700000000000002</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="Q20" s="11">
         <f t="shared" si="24"/>
-        <v>120.15</v>
+        <v>119.47</v>
       </c>
       <c r="R20" s="11">
         <f t="shared" si="24"/>
@@ -2354,19 +2354,19 @@
         <v>4</v>
       </c>
       <c r="D21">
-        <v>-14.3706387731473</v>
+        <v>-13.537492937610301</v>
       </c>
       <c r="E21">
-        <v>214.00225826595201</v>
+        <v>213.242846720866</v>
       </c>
       <c r="F21" s="12">
-        <v>3.3884420305465201E-47</v>
+        <v>4.9534089201199799E-47</v>
       </c>
       <c r="G21" s="12">
-        <v>1.26134315638926E-47</v>
+        <v>1.86330224455971E-47</v>
       </c>
       <c r="H21">
-        <v>11.3232504210564</v>
+        <v>10.9066775032879</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -2381,11 +2381,11 @@
       </c>
       <c r="M21" s="11">
         <f t="shared" si="22"/>
-        <v>-14.37</v>
+        <v>-13.54</v>
       </c>
       <c r="N21" s="11">
         <f t="shared" si="22"/>
-        <v>214</v>
+        <v>213.24</v>
       </c>
       <c r="O21" s="11">
         <f t="shared" si="23"/>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="Q21" s="11">
         <f t="shared" si="24"/>
-        <v>11.32</v>
+        <v>10.91</v>
       </c>
       <c r="R21" s="11">
         <f t="shared" si="24"/>
@@ -2415,19 +2415,19 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <v>-10.0884908268954</v>
+        <v>-7.4448560263490497</v>
       </c>
       <c r="E22">
-        <v>218.284406212204</v>
+        <v>219.33548363212699</v>
       </c>
       <c r="F22" s="12">
-        <v>3.98238687793812E-48</v>
+        <v>2.3545335682256701E-48</v>
       </c>
       <c r="G22" s="12">
-        <v>1.48243835641818E-48</v>
+        <v>8.8569463036776904E-49</v>
       </c>
       <c r="H22">
-        <v>8.1264371942696005</v>
+        <v>6.8046197939964399</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -2442,11 +2442,11 @@
       </c>
       <c r="M22" s="11">
         <f t="shared" si="22"/>
-        <v>-10.09</v>
+        <v>-7.44</v>
       </c>
       <c r="N22" s="11">
         <f t="shared" si="22"/>
-        <v>218.28</v>
+        <v>219.34</v>
       </c>
       <c r="O22" s="11">
         <f t="shared" si="23"/>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="Q22" s="11">
         <f t="shared" si="24"/>
-        <v>8.1300000000000008</v>
+        <v>6.8</v>
       </c>
       <c r="R22" s="11">
         <f t="shared" si="24"/>
@@ -2806,7 +2806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>